<commit_message>
HBIS Linelist korte korte asi
</commit_message>
<xml_diff>
--- a/Android Studio Projects/HBISLinelist/DB and Documents/hbislinelist.xlsx
+++ b/Android Studio Projects/HBISLinelist/DB and Documents/hbislinelist.xlsx
@@ -13,13 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>hhid</t>
   </si>
@@ -39,9 +40,6 @@
     <t>frmAddress</t>
   </si>
   <si>
-    <t>admissio</t>
-  </si>
-  <si>
     <t>frmPersonRelation</t>
   </si>
   <si>
@@ -51,18 +49,9 @@
     <t>frmSymptoms</t>
   </si>
   <si>
-    <t>Diagnosis</t>
-  </si>
-  <si>
-    <t>frmSymptomsOne</t>
-  </si>
-  <si>
     <t xml:space="preserve">Patient ID: </t>
   </si>
   <si>
-    <t>Purpose of interaction(Other)</t>
-  </si>
-  <si>
     <t>SLNo</t>
   </si>
   <si>
@@ -130,13 +119,79 @@
   </si>
   <si>
     <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>admission</t>
+  </si>
+  <si>
+    <t>sampleCollection</t>
+  </si>
+  <si>
+    <t>frmsinglechoice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample collected? </t>
+  </si>
+  <si>
+    <t>qID</t>
+  </si>
+  <si>
+    <t>CaptionEng</t>
+  </si>
+  <si>
+    <t>CaptionBang</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>qnext</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>Reason for not collecting sample</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>frmnumerictwo</t>
+  </si>
+  <si>
+    <t>sampleYes</t>
+  </si>
+  <si>
+    <t>1.Onset crosses 7 days at the time of enrollment</t>
+  </si>
+  <si>
+    <t>9. Others</t>
+  </si>
+  <si>
+    <t>reasonOther</t>
+  </si>
+  <si>
+    <t>frmtext</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +223,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="SutonnyMJ"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -183,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -206,8 +289,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="497">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -224,8 +337,489 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -248,24 +842,550 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="497">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="51"/>
+    <cellStyle name="Normal 10 2" xfId="246"/>
+    <cellStyle name="Normal 10 3" xfId="286"/>
+    <cellStyle name="Normal 11" xfId="136"/>
+    <cellStyle name="Normal 11 2" xfId="486"/>
+    <cellStyle name="Normal 11 3" xfId="480"/>
+    <cellStyle name="Normal 11 4" xfId="488"/>
+    <cellStyle name="Normal 11 5" xfId="482"/>
+    <cellStyle name="Normal 11 6" xfId="485"/>
+    <cellStyle name="Normal 12" xfId="40"/>
+    <cellStyle name="Normal 13" xfId="42"/>
+    <cellStyle name="Normal 14" xfId="139"/>
+    <cellStyle name="Normal 15" xfId="163"/>
+    <cellStyle name="Normal 15 10" xfId="330"/>
+    <cellStyle name="Normal 15 11" xfId="311"/>
+    <cellStyle name="Normal 15 12" xfId="344"/>
+    <cellStyle name="Normal 15 13" xfId="326"/>
+    <cellStyle name="Normal 15 14" xfId="331"/>
+    <cellStyle name="Normal 15 15" xfId="380"/>
+    <cellStyle name="Normal 15 16" xfId="389"/>
+    <cellStyle name="Normal 15 17" xfId="390"/>
+    <cellStyle name="Normal 15 18" xfId="394"/>
+    <cellStyle name="Normal 15 19" xfId="328"/>
+    <cellStyle name="Normal 15 2" xfId="391"/>
+    <cellStyle name="Normal 15 20" xfId="362"/>
+    <cellStyle name="Normal 15 21" xfId="317"/>
+    <cellStyle name="Normal 15 22" xfId="373"/>
+    <cellStyle name="Normal 15 23" xfId="363"/>
+    <cellStyle name="Normal 15 24" xfId="397"/>
+    <cellStyle name="Normal 15 25" xfId="347"/>
+    <cellStyle name="Normal 15 26" xfId="293"/>
+    <cellStyle name="Normal 15 27" xfId="342"/>
+    <cellStyle name="Normal 15 28" xfId="384"/>
+    <cellStyle name="Normal 15 29" xfId="370"/>
+    <cellStyle name="Normal 15 3" xfId="335"/>
+    <cellStyle name="Normal 15 30" xfId="354"/>
+    <cellStyle name="Normal 15 31" xfId="323"/>
+    <cellStyle name="Normal 15 32" xfId="350"/>
+    <cellStyle name="Normal 15 33" xfId="306"/>
+    <cellStyle name="Normal 15 34" xfId="377"/>
+    <cellStyle name="Normal 15 35" xfId="379"/>
+    <cellStyle name="Normal 15 36" xfId="298"/>
+    <cellStyle name="Normal 15 37" xfId="388"/>
+    <cellStyle name="Normal 15 38" xfId="302"/>
+    <cellStyle name="Normal 15 39" xfId="299"/>
+    <cellStyle name="Normal 15 4" xfId="313"/>
+    <cellStyle name="Normal 15 40" xfId="297"/>
+    <cellStyle name="Normal 15 41" xfId="336"/>
+    <cellStyle name="Normal 15 42" xfId="310"/>
+    <cellStyle name="Normal 15 43" xfId="316"/>
+    <cellStyle name="Normal 15 44" xfId="357"/>
+    <cellStyle name="Normal 15 45" xfId="402"/>
+    <cellStyle name="Normal 15 46" xfId="368"/>
+    <cellStyle name="Normal 15 47" xfId="356"/>
+    <cellStyle name="Normal 15 48" xfId="400"/>
+    <cellStyle name="Normal 15 49" xfId="348"/>
+    <cellStyle name="Normal 15 5" xfId="369"/>
+    <cellStyle name="Normal 15 50" xfId="382"/>
+    <cellStyle name="Normal 15 51" xfId="324"/>
+    <cellStyle name="Normal 15 52" xfId="295"/>
+    <cellStyle name="Normal 15 53" xfId="359"/>
+    <cellStyle name="Normal 15 54" xfId="408"/>
+    <cellStyle name="Normal 15 55" xfId="403"/>
+    <cellStyle name="Normal 15 56" xfId="304"/>
+    <cellStyle name="Normal 15 57" xfId="329"/>
+    <cellStyle name="Normal 15 58" xfId="305"/>
+    <cellStyle name="Normal 15 59" xfId="340"/>
+    <cellStyle name="Normal 15 6" xfId="361"/>
+    <cellStyle name="Normal 15 60" xfId="424"/>
+    <cellStyle name="Normal 15 61" xfId="430"/>
+    <cellStyle name="Normal 15 62" xfId="422"/>
+    <cellStyle name="Normal 15 63" xfId="414"/>
+    <cellStyle name="Normal 15 64" xfId="413"/>
+    <cellStyle name="Normal 15 65" xfId="417"/>
+    <cellStyle name="Normal 15 66" xfId="419"/>
+    <cellStyle name="Normal 15 67" xfId="420"/>
+    <cellStyle name="Normal 15 68" xfId="418"/>
+    <cellStyle name="Normal 15 69" xfId="421"/>
+    <cellStyle name="Normal 15 7" xfId="314"/>
+    <cellStyle name="Normal 15 70" xfId="416"/>
+    <cellStyle name="Normal 15 71" xfId="469"/>
+    <cellStyle name="Normal 15 72" xfId="470"/>
+    <cellStyle name="Normal 15 73" xfId="474"/>
+    <cellStyle name="Normal 15 74" xfId="473"/>
+    <cellStyle name="Normal 15 75" xfId="475"/>
+    <cellStyle name="Normal 15 76" xfId="471"/>
+    <cellStyle name="Normal 15 8" xfId="332"/>
+    <cellStyle name="Normal 15 9" xfId="333"/>
+    <cellStyle name="Normal 16" xfId="208"/>
+    <cellStyle name="Normal 17" xfId="477"/>
+    <cellStyle name="Normal 18" xfId="151"/>
+    <cellStyle name="Normal 19" xfId="483"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 2 2" xfId="2"/>
+    <cellStyle name="Normal 2 2 10" xfId="210"/>
+    <cellStyle name="Normal 2 2 11" xfId="217"/>
+    <cellStyle name="Normal 2 2 12" xfId="223"/>
+    <cellStyle name="Normal 2 2 13" xfId="229"/>
+    <cellStyle name="Normal 2 2 14" xfId="235"/>
+    <cellStyle name="Normal 2 2 15" xfId="241"/>
+    <cellStyle name="Normal 2 2 2" xfId="20"/>
+    <cellStyle name="Normal 2 2 3" xfId="27"/>
+    <cellStyle name="Normal 2 2 4" xfId="177"/>
+    <cellStyle name="Normal 2 2 5" xfId="183"/>
+    <cellStyle name="Normal 2 2 6" xfId="188"/>
+    <cellStyle name="Normal 2 2 7" xfId="193"/>
+    <cellStyle name="Normal 2 2 8" xfId="199"/>
+    <cellStyle name="Normal 2 2 9" xfId="198"/>
     <cellStyle name="Normal 2 3" xfId="6"/>
+    <cellStyle name="Normal 2 3 10" xfId="211"/>
+    <cellStyle name="Normal 2 3 11" xfId="218"/>
+    <cellStyle name="Normal 2 3 12" xfId="224"/>
+    <cellStyle name="Normal 2 3 13" xfId="230"/>
+    <cellStyle name="Normal 2 3 14" xfId="236"/>
+    <cellStyle name="Normal 2 3 15" xfId="242"/>
+    <cellStyle name="Normal 2 3 2" xfId="21"/>
+    <cellStyle name="Normal 2 3 3" xfId="28"/>
+    <cellStyle name="Normal 2 3 4" xfId="178"/>
+    <cellStyle name="Normal 2 3 5" xfId="184"/>
+    <cellStyle name="Normal 2 3 6" xfId="189"/>
+    <cellStyle name="Normal 2 3 7" xfId="194"/>
+    <cellStyle name="Normal 2 3 8" xfId="200"/>
+    <cellStyle name="Normal 2 3 9" xfId="204"/>
     <cellStyle name="Normal 2 4" xfId="8"/>
+    <cellStyle name="Normal 2 4 10" xfId="213"/>
+    <cellStyle name="Normal 2 4 11" xfId="220"/>
+    <cellStyle name="Normal 2 4 12" xfId="226"/>
+    <cellStyle name="Normal 2 4 13" xfId="232"/>
+    <cellStyle name="Normal 2 4 14" xfId="238"/>
+    <cellStyle name="Normal 2 4 15" xfId="244"/>
+    <cellStyle name="Normal 2 4 2" xfId="23"/>
+    <cellStyle name="Normal 2 4 3" xfId="30"/>
+    <cellStyle name="Normal 2 4 4" xfId="180"/>
+    <cellStyle name="Normal 2 4 5" xfId="186"/>
+    <cellStyle name="Normal 2 4 6" xfId="191"/>
+    <cellStyle name="Normal 2 4 7" xfId="196"/>
+    <cellStyle name="Normal 2 4 8" xfId="202"/>
+    <cellStyle name="Normal 2 4 9" xfId="206"/>
     <cellStyle name="Normal 2 5" xfId="15"/>
+    <cellStyle name="Normal 2 6" xfId="16"/>
+    <cellStyle name="Normal 2 7" xfId="34"/>
+    <cellStyle name="Normal 20" xfId="154"/>
+    <cellStyle name="Normal 21" xfId="156"/>
+    <cellStyle name="Normal 22" xfId="152"/>
+    <cellStyle name="Normal 22 10" xfId="360"/>
+    <cellStyle name="Normal 22 100" xfId="439"/>
+    <cellStyle name="Normal 22 101" xfId="445"/>
+    <cellStyle name="Normal 22 102" xfId="450"/>
+    <cellStyle name="Normal 22 103" xfId="456"/>
+    <cellStyle name="Normal 22 104" xfId="458"/>
+    <cellStyle name="Normal 22 105" xfId="457"/>
+    <cellStyle name="Normal 22 106" xfId="291"/>
+    <cellStyle name="Normal 22 107" xfId="460"/>
+    <cellStyle name="Normal 22 108" xfId="459"/>
+    <cellStyle name="Normal 22 109" xfId="461"/>
+    <cellStyle name="Normal 22 11" xfId="353"/>
+    <cellStyle name="Normal 22 110" xfId="462"/>
+    <cellStyle name="Normal 22 111" xfId="463"/>
+    <cellStyle name="Normal 22 112" xfId="465"/>
+    <cellStyle name="Normal 22 113" xfId="464"/>
+    <cellStyle name="Normal 22 114" xfId="466"/>
+    <cellStyle name="Normal 22 115" xfId="468"/>
+    <cellStyle name="Normal 22 116" xfId="476"/>
+    <cellStyle name="Normal 22 117" xfId="472"/>
+    <cellStyle name="Normal 22 118" xfId="467"/>
+    <cellStyle name="Normal 22 12" xfId="343"/>
+    <cellStyle name="Normal 22 13" xfId="372"/>
+    <cellStyle name="Normal 22 14" xfId="386"/>
+    <cellStyle name="Normal 22 15" xfId="309"/>
+    <cellStyle name="Normal 22 16" xfId="334"/>
+    <cellStyle name="Normal 22 17" xfId="346"/>
+    <cellStyle name="Normal 22 18" xfId="308"/>
+    <cellStyle name="Normal 22 19" xfId="318"/>
+    <cellStyle name="Normal 22 2" xfId="162"/>
+    <cellStyle name="Normal 22 20" xfId="387"/>
+    <cellStyle name="Normal 22 21" xfId="320"/>
+    <cellStyle name="Normal 22 22" xfId="375"/>
+    <cellStyle name="Normal 22 23" xfId="307"/>
+    <cellStyle name="Normal 22 24" xfId="339"/>
+    <cellStyle name="Normal 22 25" xfId="294"/>
+    <cellStyle name="Normal 22 26" xfId="325"/>
+    <cellStyle name="Normal 22 27" xfId="300"/>
+    <cellStyle name="Normal 22 28" xfId="341"/>
+    <cellStyle name="Normal 22 29" xfId="381"/>
+    <cellStyle name="Normal 22 3" xfId="161"/>
+    <cellStyle name="Normal 22 30" xfId="401"/>
+    <cellStyle name="Normal 22 31" xfId="352"/>
+    <cellStyle name="Normal 22 32" xfId="398"/>
+    <cellStyle name="Normal 22 33" xfId="345"/>
+    <cellStyle name="Normal 22 34" xfId="364"/>
+    <cellStyle name="Normal 22 35" xfId="338"/>
+    <cellStyle name="Normal 22 36" xfId="322"/>
+    <cellStyle name="Normal 22 37" xfId="366"/>
+    <cellStyle name="Normal 22 38" xfId="376"/>
+    <cellStyle name="Normal 22 39" xfId="396"/>
+    <cellStyle name="Normal 22 4" xfId="160"/>
+    <cellStyle name="Normal 22 40" xfId="383"/>
+    <cellStyle name="Normal 22 41" xfId="404"/>
+    <cellStyle name="Normal 22 42" xfId="393"/>
+    <cellStyle name="Normal 22 43" xfId="406"/>
+    <cellStyle name="Normal 22 44" xfId="405"/>
+    <cellStyle name="Normal 22 45" xfId="296"/>
+    <cellStyle name="Normal 22 46" xfId="395"/>
+    <cellStyle name="Normal 22 47" xfId="385"/>
+    <cellStyle name="Normal 22 48" xfId="327"/>
+    <cellStyle name="Normal 22 49" xfId="365"/>
+    <cellStyle name="Normal 22 5" xfId="288"/>
+    <cellStyle name="Normal 22 50" xfId="312"/>
+    <cellStyle name="Normal 22 51" xfId="367"/>
+    <cellStyle name="Normal 22 52" xfId="303"/>
+    <cellStyle name="Normal 22 53" xfId="349"/>
+    <cellStyle name="Normal 22 54" xfId="351"/>
+    <cellStyle name="Normal 22 55" xfId="321"/>
+    <cellStyle name="Normal 22 56" xfId="315"/>
+    <cellStyle name="Normal 22 57" xfId="392"/>
+    <cellStyle name="Normal 22 58" xfId="399"/>
+    <cellStyle name="Normal 22 59" xfId="371"/>
+    <cellStyle name="Normal 22 6" xfId="290"/>
+    <cellStyle name="Normal 22 60" xfId="355"/>
+    <cellStyle name="Normal 22 61" xfId="301"/>
+    <cellStyle name="Normal 22 62" xfId="374"/>
+    <cellStyle name="Normal 22 63" xfId="378"/>
+    <cellStyle name="Normal 22 64" xfId="358"/>
+    <cellStyle name="Normal 22 65" xfId="409"/>
+    <cellStyle name="Normal 22 66" xfId="407"/>
+    <cellStyle name="Normal 22 67" xfId="319"/>
+    <cellStyle name="Normal 22 68" xfId="423"/>
+    <cellStyle name="Normal 22 69" xfId="412"/>
+    <cellStyle name="Normal 22 7" xfId="289"/>
+    <cellStyle name="Normal 22 70" xfId="425"/>
+    <cellStyle name="Normal 22 71" xfId="428"/>
+    <cellStyle name="Normal 22 72" xfId="431"/>
+    <cellStyle name="Normal 22 73" xfId="410"/>
+    <cellStyle name="Normal 22 74" xfId="429"/>
+    <cellStyle name="Normal 22 75" xfId="426"/>
+    <cellStyle name="Normal 22 76" xfId="427"/>
+    <cellStyle name="Normal 22 77" xfId="411"/>
+    <cellStyle name="Normal 22 78" xfId="415"/>
+    <cellStyle name="Normal 22 79" xfId="444"/>
+    <cellStyle name="Normal 22 8" xfId="292"/>
+    <cellStyle name="Normal 22 80" xfId="436"/>
+    <cellStyle name="Normal 22 81" xfId="447"/>
+    <cellStyle name="Normal 22 82" xfId="451"/>
+    <cellStyle name="Normal 22 83" xfId="455"/>
+    <cellStyle name="Normal 22 84" xfId="435"/>
+    <cellStyle name="Normal 22 85" xfId="442"/>
+    <cellStyle name="Normal 22 86" xfId="446"/>
+    <cellStyle name="Normal 22 87" xfId="441"/>
+    <cellStyle name="Normal 22 88" xfId="438"/>
+    <cellStyle name="Normal 22 89" xfId="453"/>
+    <cellStyle name="Normal 22 9" xfId="337"/>
+    <cellStyle name="Normal 22 90" xfId="449"/>
+    <cellStyle name="Normal 22 91" xfId="434"/>
+    <cellStyle name="Normal 22 92" xfId="433"/>
+    <cellStyle name="Normal 22 93" xfId="440"/>
+    <cellStyle name="Normal 22 94" xfId="443"/>
+    <cellStyle name="Normal 22 95" xfId="452"/>
+    <cellStyle name="Normal 22 96" xfId="432"/>
+    <cellStyle name="Normal 22 97" xfId="437"/>
+    <cellStyle name="Normal 22 98" xfId="454"/>
+    <cellStyle name="Normal 22 99" xfId="448"/>
+    <cellStyle name="Normal 23" xfId="489"/>
+    <cellStyle name="Normal 24" xfId="484"/>
+    <cellStyle name="Normal 25" xfId="479"/>
     <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 3 10" xfId="43"/>
+    <cellStyle name="Normal 3 11" xfId="45"/>
+    <cellStyle name="Normal 3 12" xfId="47"/>
+    <cellStyle name="Normal 3 13" xfId="50"/>
+    <cellStyle name="Normal 3 14" xfId="53"/>
+    <cellStyle name="Normal 3 15" xfId="55"/>
+    <cellStyle name="Normal 3 16" xfId="69"/>
+    <cellStyle name="Normal 3 17" xfId="76"/>
+    <cellStyle name="Normal 3 18" xfId="83"/>
+    <cellStyle name="Normal 3 19" xfId="90"/>
     <cellStyle name="Normal 3 2" xfId="10"/>
+    <cellStyle name="Normal 3 20" xfId="97"/>
+    <cellStyle name="Normal 3 21" xfId="104"/>
+    <cellStyle name="Normal 3 22" xfId="111"/>
+    <cellStyle name="Normal 3 23" xfId="117"/>
+    <cellStyle name="Normal 3 24" xfId="123"/>
+    <cellStyle name="Normal 3 25" xfId="128"/>
+    <cellStyle name="Normal 3 26" xfId="131"/>
+    <cellStyle name="Normal 3 27" xfId="135"/>
+    <cellStyle name="Normal 3 28" xfId="137"/>
+    <cellStyle name="Normal 3 29" xfId="138"/>
+    <cellStyle name="Normal 3 3" xfId="18"/>
+    <cellStyle name="Normal 3 30" xfId="141"/>
+    <cellStyle name="Normal 3 4" xfId="26"/>
+    <cellStyle name="Normal 3 5" xfId="37"/>
+    <cellStyle name="Normal 3 6" xfId="35"/>
+    <cellStyle name="Normal 3 7" xfId="38"/>
+    <cellStyle name="Normal 3 8" xfId="39"/>
+    <cellStyle name="Normal 3 9" xfId="41"/>
     <cellStyle name="Normal 4" xfId="4"/>
     <cellStyle name="Normal 5" xfId="5"/>
+    <cellStyle name="Normal 5 10" xfId="96"/>
+    <cellStyle name="Normal 5 10 2" xfId="209"/>
+    <cellStyle name="Normal 5 10 2 2" xfId="270"/>
+    <cellStyle name="Normal 5 10 3" xfId="261"/>
+    <cellStyle name="Normal 5 10 4" xfId="254"/>
+    <cellStyle name="Normal 5 11" xfId="103"/>
+    <cellStyle name="Normal 5 11 2" xfId="216"/>
+    <cellStyle name="Normal 5 11 3" xfId="276"/>
+    <cellStyle name="Normal 5 12" xfId="110"/>
+    <cellStyle name="Normal 5 12 2" xfId="222"/>
+    <cellStyle name="Normal 5 12 3" xfId="278"/>
+    <cellStyle name="Normal 5 13" xfId="116"/>
+    <cellStyle name="Normal 5 13 2" xfId="228"/>
+    <cellStyle name="Normal 5 13 3" xfId="280"/>
+    <cellStyle name="Normal 5 14" xfId="122"/>
+    <cellStyle name="Normal 5 14 2" xfId="234"/>
+    <cellStyle name="Normal 5 14 3" xfId="282"/>
+    <cellStyle name="Normal 5 15" xfId="127"/>
+    <cellStyle name="Normal 5 15 2" xfId="240"/>
+    <cellStyle name="Normal 5 15 3" xfId="284"/>
+    <cellStyle name="Normal 5 16" xfId="134"/>
+    <cellStyle name="Normal 5 17" xfId="133"/>
+    <cellStyle name="Normal 5 18" xfId="140"/>
+    <cellStyle name="Normal 5 19" xfId="142"/>
     <cellStyle name="Normal 5 2" xfId="7"/>
+    <cellStyle name="Normal 5 2 10" xfId="95"/>
+    <cellStyle name="Normal 5 2 10 2" xfId="219"/>
+    <cellStyle name="Normal 5 2 10 3" xfId="277"/>
+    <cellStyle name="Normal 5 2 11" xfId="102"/>
+    <cellStyle name="Normal 5 2 11 2" xfId="225"/>
+    <cellStyle name="Normal 5 2 11 3" xfId="279"/>
+    <cellStyle name="Normal 5 2 12" xfId="109"/>
+    <cellStyle name="Normal 5 2 12 2" xfId="231"/>
+    <cellStyle name="Normal 5 2 12 3" xfId="281"/>
+    <cellStyle name="Normal 5 2 13" xfId="115"/>
+    <cellStyle name="Normal 5 2 13 2" xfId="237"/>
+    <cellStyle name="Normal 5 2 13 3" xfId="283"/>
+    <cellStyle name="Normal 5 2 14" xfId="121"/>
+    <cellStyle name="Normal 5 2 14 2" xfId="243"/>
+    <cellStyle name="Normal 5 2 14 3" xfId="285"/>
+    <cellStyle name="Normal 5 2 15" xfId="126"/>
+    <cellStyle name="Normal 5 2 2" xfId="19"/>
+    <cellStyle name="Normal 5 2 2 10" xfId="93"/>
+    <cellStyle name="Normal 5 2 2 11" xfId="100"/>
+    <cellStyle name="Normal 5 2 2 12" xfId="107"/>
+    <cellStyle name="Normal 5 2 2 13" xfId="113"/>
+    <cellStyle name="Normal 5 2 2 14" xfId="119"/>
+    <cellStyle name="Normal 5 2 2 2" xfId="22"/>
+    <cellStyle name="Normal 5 2 2 3" xfId="63"/>
+    <cellStyle name="Normal 5 2 2 3 2" xfId="262"/>
+    <cellStyle name="Normal 5 2 2 3 3" xfId="287"/>
+    <cellStyle name="Normal 5 2 2 4" xfId="61"/>
+    <cellStyle name="Normal 5 2 2 5" xfId="48"/>
+    <cellStyle name="Normal 5 2 2 6" xfId="65"/>
+    <cellStyle name="Normal 5 2 2 7" xfId="72"/>
+    <cellStyle name="Normal 5 2 2 8" xfId="79"/>
+    <cellStyle name="Normal 5 2 2 9" xfId="86"/>
+    <cellStyle name="Normal 5 2 3" xfId="29"/>
+    <cellStyle name="Normal 5 2 4" xfId="60"/>
+    <cellStyle name="Normal 5 2 4 2" xfId="179"/>
+    <cellStyle name="Normal 5 2 4 3" xfId="215"/>
+    <cellStyle name="Normal 5 2 5" xfId="62"/>
+    <cellStyle name="Normal 5 2 5 2" xfId="185"/>
+    <cellStyle name="Normal 5 2 5 3" xfId="175"/>
+    <cellStyle name="Normal 5 2 6" xfId="67"/>
+    <cellStyle name="Normal 5 2 6 2" xfId="190"/>
+    <cellStyle name="Normal 5 2 6 3" xfId="271"/>
+    <cellStyle name="Normal 5 2 7" xfId="74"/>
+    <cellStyle name="Normal 5 2 7 2" xfId="195"/>
+    <cellStyle name="Normal 5 2 7 3" xfId="272"/>
+    <cellStyle name="Normal 5 2 8" xfId="81"/>
+    <cellStyle name="Normal 5 2 8 2" xfId="201"/>
+    <cellStyle name="Normal 5 2 8 3" xfId="273"/>
+    <cellStyle name="Normal 5 2 9" xfId="88"/>
+    <cellStyle name="Normal 5 2 9 2" xfId="212"/>
+    <cellStyle name="Normal 5 2 9 3" xfId="275"/>
+    <cellStyle name="Normal 5 20" xfId="143"/>
+    <cellStyle name="Normal 5 21" xfId="144"/>
+    <cellStyle name="Normal 5 22" xfId="145"/>
+    <cellStyle name="Normal 5 23" xfId="146"/>
+    <cellStyle name="Normal 5 24" xfId="147"/>
+    <cellStyle name="Normal 5 25" xfId="148"/>
+    <cellStyle name="Normal 5 26" xfId="149"/>
+    <cellStyle name="Normal 5 27" xfId="150"/>
+    <cellStyle name="Normal 5 28" xfId="153"/>
+    <cellStyle name="Normal 5 29" xfId="155"/>
     <cellStyle name="Normal 5 3" xfId="13"/>
+    <cellStyle name="Normal 5 3 10" xfId="114"/>
+    <cellStyle name="Normal 5 3 11" xfId="120"/>
+    <cellStyle name="Normal 5 3 12" xfId="125"/>
+    <cellStyle name="Normal 5 3 13" xfId="130"/>
+    <cellStyle name="Normal 5 3 14" xfId="132"/>
+    <cellStyle name="Normal 5 3 15" xfId="164"/>
+    <cellStyle name="Normal 5 3 16" xfId="182"/>
+    <cellStyle name="Normal 5 3 2" xfId="44"/>
+    <cellStyle name="Normal 5 3 2 2" xfId="57"/>
+    <cellStyle name="Normal 5 3 3" xfId="66"/>
+    <cellStyle name="Normal 5 3 3 2" xfId="255"/>
+    <cellStyle name="Normal 5 3 4" xfId="73"/>
+    <cellStyle name="Normal 5 3 4 2" xfId="257"/>
+    <cellStyle name="Normal 5 3 5" xfId="80"/>
+    <cellStyle name="Normal 5 3 5 2" xfId="258"/>
+    <cellStyle name="Normal 5 3 6" xfId="87"/>
+    <cellStyle name="Normal 5 3 6 2" xfId="259"/>
+    <cellStyle name="Normal 5 3 7" xfId="94"/>
+    <cellStyle name="Normal 5 3 7 2" xfId="260"/>
+    <cellStyle name="Normal 5 3 8" xfId="101"/>
+    <cellStyle name="Normal 5 3 8 2" xfId="263"/>
+    <cellStyle name="Normal 5 3 9" xfId="108"/>
+    <cellStyle name="Normal 5 30" xfId="157"/>
+    <cellStyle name="Normal 5 31" xfId="158"/>
+    <cellStyle name="Normal 5 32" xfId="159"/>
+    <cellStyle name="Normal 5 4" xfId="17"/>
+    <cellStyle name="Normal 5 4 2" xfId="167"/>
+    <cellStyle name="Normal 5 4 2 2" xfId="264"/>
+    <cellStyle name="Normal 5 4 3" xfId="248"/>
+    <cellStyle name="Normal 5 4 4" xfId="174"/>
+    <cellStyle name="Normal 5 4 5" xfId="487"/>
+    <cellStyle name="Normal 5 4 6" xfId="478"/>
+    <cellStyle name="Normal 5 4 7" xfId="490"/>
+    <cellStyle name="Normal 5 4 8" xfId="492"/>
+    <cellStyle name="Normal 5 4 9" xfId="494"/>
+    <cellStyle name="Normal 5 5" xfId="59"/>
+    <cellStyle name="Normal 5 5 2" xfId="165"/>
+    <cellStyle name="Normal 5 5 2 2" xfId="265"/>
+    <cellStyle name="Normal 5 5 3" xfId="249"/>
+    <cellStyle name="Normal 5 5 4" xfId="176"/>
+    <cellStyle name="Normal 5 6" xfId="68"/>
+    <cellStyle name="Normal 5 6 2" xfId="166"/>
+    <cellStyle name="Normal 5 6 2 2" xfId="266"/>
+    <cellStyle name="Normal 5 6 3" xfId="250"/>
+    <cellStyle name="Normal 5 6 4" xfId="247"/>
+    <cellStyle name="Normal 5 7" xfId="75"/>
+    <cellStyle name="Normal 5 7 2" xfId="168"/>
+    <cellStyle name="Normal 5 7 2 2" xfId="267"/>
+    <cellStyle name="Normal 5 7 3" xfId="251"/>
+    <cellStyle name="Normal 5 7 4" xfId="173"/>
+    <cellStyle name="Normal 5 8" xfId="82"/>
+    <cellStyle name="Normal 5 8 2" xfId="169"/>
+    <cellStyle name="Normal 5 8 2 2" xfId="268"/>
+    <cellStyle name="Normal 5 8 3" xfId="252"/>
+    <cellStyle name="Normal 5 8 4" xfId="172"/>
+    <cellStyle name="Normal 5 9" xfId="89"/>
+    <cellStyle name="Normal 5 9 2" xfId="171"/>
+    <cellStyle name="Normal 5 9 2 2" xfId="205"/>
+    <cellStyle name="Normal 5 9 2 3" xfId="274"/>
+    <cellStyle name="Normal 5 9 3" xfId="256"/>
+    <cellStyle name="Normal 5 9 4" xfId="170"/>
     <cellStyle name="Normal 6" xfId="9"/>
+    <cellStyle name="Normal 6 10" xfId="214"/>
+    <cellStyle name="Normal 6 11" xfId="221"/>
+    <cellStyle name="Normal 6 12" xfId="227"/>
+    <cellStyle name="Normal 6 13" xfId="233"/>
+    <cellStyle name="Normal 6 14" xfId="239"/>
+    <cellStyle name="Normal 6 15" xfId="245"/>
+    <cellStyle name="Normal 6 2" xfId="24"/>
+    <cellStyle name="Normal 6 3" xfId="31"/>
+    <cellStyle name="Normal 6 4" xfId="181"/>
+    <cellStyle name="Normal 6 5" xfId="187"/>
+    <cellStyle name="Normal 6 6" xfId="192"/>
+    <cellStyle name="Normal 6 7" xfId="197"/>
+    <cellStyle name="Normal 6 8" xfId="203"/>
+    <cellStyle name="Normal 6 9" xfId="207"/>
     <cellStyle name="Normal 7" xfId="12"/>
+    <cellStyle name="Normal 7 10" xfId="77"/>
+    <cellStyle name="Normal 7 11" xfId="84"/>
+    <cellStyle name="Normal 7 12" xfId="91"/>
+    <cellStyle name="Normal 7 13" xfId="98"/>
+    <cellStyle name="Normal 7 14" xfId="105"/>
+    <cellStyle name="Normal 7 15" xfId="481"/>
+    <cellStyle name="Normal 7 16" xfId="491"/>
+    <cellStyle name="Normal 7 17" xfId="493"/>
+    <cellStyle name="Normal 7 18" xfId="495"/>
+    <cellStyle name="Normal 7 19" xfId="496"/>
+    <cellStyle name="Normal 7 2" xfId="33"/>
+    <cellStyle name="Normal 7 3" xfId="58"/>
+    <cellStyle name="Normal 7 4" xfId="46"/>
+    <cellStyle name="Normal 7 5" xfId="49"/>
+    <cellStyle name="Normal 7 6" xfId="64"/>
+    <cellStyle name="Normal 7 7" xfId="56"/>
+    <cellStyle name="Normal 7 8" xfId="52"/>
+    <cellStyle name="Normal 7 9" xfId="70"/>
     <cellStyle name="Normal 8" xfId="11"/>
+    <cellStyle name="Normal 8 10" xfId="106"/>
+    <cellStyle name="Normal 8 11" xfId="112"/>
+    <cellStyle name="Normal 8 12" xfId="118"/>
+    <cellStyle name="Normal 8 13" xfId="124"/>
+    <cellStyle name="Normal 8 14" xfId="129"/>
+    <cellStyle name="Normal 8 2" xfId="25"/>
+    <cellStyle name="Normal 8 2 2" xfId="32"/>
+    <cellStyle name="Normal 8 3" xfId="36"/>
+    <cellStyle name="Normal 8 4" xfId="54"/>
+    <cellStyle name="Normal 8 5" xfId="71"/>
+    <cellStyle name="Normal 8 6" xfId="78"/>
+    <cellStyle name="Normal 8 7" xfId="85"/>
+    <cellStyle name="Normal 8 8" xfId="92"/>
+    <cellStyle name="Normal 8 9" xfId="99"/>
     <cellStyle name="Normal 9" xfId="14"/>
+    <cellStyle name="Normal 9 2" xfId="269"/>
+    <cellStyle name="Normal 9 3" xfId="253"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -557,10 +1677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U87"/>
+  <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -576,64 +1696,64 @@
   <sheetData>
     <row r="1" spans="1:21" ht="25.5">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="R1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="S1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="T1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -647,31 +1767,31 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>2</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="U2" t="str">
         <f>"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A2&amp;"', '" &amp;B2&amp;"','" &amp;C2&amp;"', '" &amp;D2&amp;"','" &amp;E2&amp;"','" &amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"', '"&amp;K2&amp;"','"&amp;L2&amp;"','"&amp;M2&amp;"','"&amp;N2&amp;"','"&amp;O2&amp;"','"&amp;P2&amp;"','"&amp;Q2&amp;"',"&amp;R2&amp;","&amp;S2&amp;",'"&amp;T2&amp;"');"</f>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('1', 'hhid','FrmDataID', 'tblMainques','','Patient ID: ','qIdentity','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('1', 'hhid','FrmDataID', 'tblMainques','','Patient ID: ','','qIdentity','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -680,29 +1800,29 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U3" t="str">
-        <f t="shared" ref="U3:U7" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('3', 'qIdentity','frmMultipleChoiceText', 'tblMainques','','','personal','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>32</v>
+      </c>
+      <c r="U3" s="24" t="str">
+        <f t="shared" ref="U3:U10" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'qIdentity','frmMultipleChoiceText', 'tblMainques','','','','personal','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4">
-        <v>4</v>
+      <c r="A4" s="24">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -711,129 +1831,217 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="H4" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('3', 'personal','frmAddress', 'tblMainques','','','','admission','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U5" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'admission','frmPersonRelation', 'tblMainques','','','','Symptoms','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="H6" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" t="s">
+      <c r="R6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U6" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('5', 'Symptoms','frmSymptoms', 'tblMainques','','','','sampleCollection','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="24">
         <v>6</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U7" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('6', 'sampleCollection','frmsinglechoice', 'tblMainques','','Sample collected? ','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="11" customFormat="1">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U8" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'sampleYes','frmnumerictwo', 'tblMainques','','','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="30">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U4" t="str">
+      <c r="D9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U9" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'personal','frmAddress', 'tblMainques','','','admissio','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U5" t="str">
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'reason','frmsinglechoice', 'tblMainques','','Reason for not collecting sample','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U10" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('6', 'admissio','frmPersonRelation', 'tblMainques','','','Symptoms','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U6" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'Symptoms','frmSymptoms', 'tblMainques','','','Diagnosis','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="U7" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'Diagnosis','frmSymptomsOne', 'tblMainques','','Purpose of interaction(Other)','','','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="C8" s="1"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="C9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="C10" s="1"/>
-      <c r="F10" s="1"/>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'reasonOther','frmtext', 'tblMainques','','Other','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="C11" s="1"/>
@@ -1129,6 +2337,7 @@
     </row>
     <row r="84" spans="3:6">
       <c r="C84" s="1"/>
+      <c r="F84" s="1"/>
     </row>
     <row r="85" spans="3:6">
       <c r="C85" s="1"/>
@@ -1138,6 +2347,9 @@
     </row>
     <row r="87" spans="3:6">
       <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="3:6">
+      <c r="C88" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:T1"/>
@@ -1148,12 +2360,130 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="21"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75">
+      <c r="A1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15" t="str">
+        <f>"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A2&amp;"','" &amp;B2&amp;"', '" &amp;C2&amp;"','" &amp;D2&amp;"','" &amp;E2&amp;"','"&amp;F2&amp;"');"</f>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('1','sampleCollection', 'Yes','','1','sampleYes');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="21">
+        <v>2</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="15" t="str">
+        <f t="shared" ref="H3:H5" si="0">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;C3&amp;"','" &amp;D3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('2','sampleCollection', 'NO','','2','reason');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="21">
+        <v>1</v>
+      </c>
+      <c r="H4" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('3','reason', '1.Onset crosses 7 days at the time of enrollment','','1','');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75">
+      <c r="A5" s="17">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="21">
+        <v>9</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('4','reason', '9. Others','','9','reasonOther');</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Cleanliness and Toilet user added Hbis Line list also added
</commit_message>
<xml_diff>
--- a/Android Studio Projects/HBISLinelist/DB and Documents/hbislinelist.xlsx
+++ b/Android Studio Projects/HBISLinelist/DB and Documents/hbislinelist.xlsx
@@ -112,9 +112,6 @@
     <t>DataType</t>
   </si>
   <si>
-    <t>tblMainques</t>
-  </si>
-  <si>
     <t>NULL</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>END</t>
   </si>
   <si>
-    <t>frmnumerictwo</t>
-  </si>
-  <si>
     <t>sampleYes</t>
   </si>
   <si>
@@ -185,6 +179,12 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>FrmDataID2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tblLinelist </t>
   </si>
 </sst>
 </file>
@@ -819,7 +819,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -881,9 +881,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1680,7 +1677,7 @@
   <dimension ref="A1:U88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1766,8 +1763,8 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
+      <c r="D2" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
@@ -1776,17 +1773,17 @@
         <v>2</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="U2" t="str">
-        <f>"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A2&amp;"', '" &amp;B2&amp;"','" &amp;C2&amp;"', '" &amp;D2&amp;"','" &amp;E2&amp;"','" &amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"', '"&amp;K2&amp;"','"&amp;L2&amp;"','"&amp;M2&amp;"','"&amp;N2&amp;"','"&amp;O2&amp;"','"&amp;P2&amp;"','"&amp;Q2&amp;"',"&amp;R2&amp;","&amp;S2&amp;",'"&amp;T2&amp;"');"</f>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('1', 'hhid','FrmDataID', 'tblMainques','','Patient ID: ','','qIdentity','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <f>"insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A2&amp;"', '" &amp;B2&amp;"','" &amp;C2&amp;"', '" &amp;D2&amp;"','" &amp;E2&amp;"','" &amp;F2&amp;"','"&amp;G2&amp;"','"&amp;H2&amp;"','"&amp;I2&amp;"','"&amp;J2&amp;"', '"&amp;K2&amp;"','"&amp;L2&amp;"','"&amp;M2&amp;"','"&amp;N2&amp;"','"&amp;O2&amp;"','"&amp;P2&amp;"','"&amp;Q2&amp;"',"&amp;R2&amp;","&amp;S2&amp;",'"&amp;T2&amp;"');"</f>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('1', 'hhid','FrmDataID', 'tblLinelist ','','Patient ID: ','','qIdentity','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1799,25 +1796,25 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
+      <c r="D3" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="F3" s="1"/>
       <c r="H3" t="s">
         <v>4</v>
       </c>
       <c r="R3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="S3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="U3" s="24" t="str">
-        <f t="shared" ref="U3:U10" si="0">"insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'qIdentity','frmMultipleChoiceText', 'tblMainques','','','','personal','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <f t="shared" ref="U3:U10" si="0">"insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('" &amp;A3&amp;"', '" &amp;B3&amp;"','" &amp;C3&amp;"', '" &amp;D3&amp;"','" &amp;E3&amp;"','" &amp;F3&amp;"','"&amp;G3&amp;"','"&amp;H3&amp;"','"&amp;I3&amp;"','"&amp;J3&amp;"', '"&amp;K3&amp;"','"&amp;L3&amp;"','"&amp;M3&amp;"','"&amp;N3&amp;"','"&amp;O3&amp;"','"&amp;P3&amp;"','"&amp;Q3&amp;"',"&amp;R3&amp;","&amp;S3&amp;",'"&amp;T3&amp;"');"</f>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('2', 'qIdentity','frmMultipleChoiceText', 'tblLinelist ','','','','personal','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1827,28 +1824,28 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>30</v>
+      <c r="D4" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="F4" s="1"/>
       <c r="H4" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="U4" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('3', 'personal','frmAddress', 'tblMainques','','','','admission','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('3', 'personal','frmAddress', 'tblLinelist ','','','','admission','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1856,30 +1853,30 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>30</v>
+      <c r="D5" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="F5" s="1"/>
       <c r="H5" t="s">
         <v>7</v>
       </c>
       <c r="R5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="U5" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'admission','frmPersonRelation', 'tblMainques','','','','Symptoms','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('4', 'admission','frmPersonRelation', 'tblLinelist ','','','','Symptoms','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1892,25 +1889,25 @@
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>30</v>
+      <c r="D6" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="F6" s="1"/>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="U6" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('5', 'Symptoms','frmSymptoms', 'tblMainques','','','','sampleCollection','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('5', 'Symptoms','frmSymptoms', 'tblLinelist ','','','','sampleCollection','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1918,32 +1915,32 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="R7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="R7" s="7" t="s">
+      <c r="S7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="U7" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('6', 'sampleCollection','frmsinglechoice', 'tblMainques','','Sample collected? ','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('6', 'sampleCollection','frmsinglechoice', 'tblLinelist ','','Sample collected? ','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="11" customFormat="1">
@@ -1951,30 +1948,30 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="F8" s="2"/>
       <c r="H8" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T8" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T8" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="U8" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'sampleYes','frmnumerictwo', 'tblMainques','','','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('7', 'sampleYes','FrmDataID2', 'tblLinelist ','','','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="30">
@@ -1982,32 +1979,32 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="H9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="R9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="R9" s="7" t="s">
+      <c r="S9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T9" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="U9" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'reason','frmsinglechoice', 'tblMainques','','Reason for not collecting sample','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'reason','frmsinglechoice', 'tblLinelist ','','Reason for not collecting sample','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2015,32 +2012,32 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="24" t="s">
+      <c r="H10" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="R10" s="7" t="s">
+      <c r="S10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T10" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="U10" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'reasonOther','frmtext', 'tblMainques','','Other','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestionLList (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'reasonOther','frmtext', 'tblLinelist ','','Other','','END','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -2380,23 +2377,23 @@
         <v>10</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>41</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5">
@@ -2404,22 +2401,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="8">
         <v>1</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="15" t="str">
-        <f>"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A2&amp;"','" &amp;B2&amp;"', '" &amp;C2&amp;"','" &amp;D2&amp;"','" &amp;E2&amp;"','"&amp;F2&amp;"');"</f>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('1','sampleCollection', 'Yes','','1','sampleYes');</v>
+        <f>"insert into tblOptionsLList (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A2&amp;"','" &amp;B2&amp;"', '" &amp;C2&amp;"','" &amp;D2&amp;"','" &amp;E2&amp;"','"&amp;F2&amp;"');"</f>
+        <v>insert into tblOptionsLList (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('1','sampleCollection', 'Yes','','1','sampleYes');</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75">
@@ -2427,20 +2424,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="21">
         <v>2</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="15" t="str">
-        <f t="shared" ref="H3:H5" si="0">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;C3&amp;"','" &amp;D3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('2','sampleCollection', 'NO','','2','reason');</v>
+        <f t="shared" ref="H3:H5" si="0">"insert into tblOptionsLList (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;C3&amp;"','" &amp;D3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
+        <v>insert into tblOptionsLList (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('2','sampleCollection', 'NO','','2','reason');</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45">
@@ -2448,17 +2445,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" s="21">
         <v>1</v>
       </c>
       <c r="H4" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('3','reason', '1.Onset crosses 7 days at the time of enrollment','','1','');</v>
+        <v>insert into tblOptionsLList (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('3','reason', '1.Onset crosses 7 days at the time of enrollment','','1','');</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75">
@@ -2466,20 +2463,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" s="21">
         <v>9</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H5" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('4','reason', '9. Others','','9','reasonOther');</v>
+        <v>insert into tblOptionsLList (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('4','reason', '9. Others','','9','reasonOther');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>